<commit_message>
[UPD] alquileres.py // alquileres.xlsx : not working
</commit_message>
<xml_diff>
--- a/alquileres.xlsx
+++ b/alquileres.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Características</t>
+          <t>Precio/m²Características</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -512,6 +512,188 @@
       <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Teléfono</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Características Básicas</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Más Características</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>105773947</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alquiler</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alquiler de Ático en Peñas Negras, 12</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>('\nPeñas Negras, 12\n',)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>('\nBarrio Torreagüera\n',)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>('\nDistrito Pedanías Este\n',)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>('\nMurcia\n',)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Área de Murcia, Murcia
+</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>700€/mes</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>105773947</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Profesional</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>CITYSOL MURCIA</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Anuncio actualizado el 20 de agosto</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>['128 m² construidos', '3 habitaciones', '2 baños', 'Terraza y balcón', 'Plaza de garaje incluida en el precio', 'Segunda mano/buen estado', 'Armarios empotrados', 'Trastero', 'Orientación este, oeste', 'Construido en 2010', 'Cocina equipada y casa sin amueblar', 'Planta 3ª exterior', 'Con ascensor']</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>37324696</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Alquiler</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alquiler de Piso en calle Jacobo de las Leyes</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>('\nCalle Jacobo de las Leyes\n',)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>('\nBarrio La Fama\n',)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>('\nDistrito Centro\n',)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>('\nMurcia\n',)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Área de Murcia, Murcia
+</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>750€/mes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Fianza de 1 mes</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2530</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Profesional</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>The Simple Rent</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Anuncio actualizado el 20 de agosto</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>['90 m² construidos, 85 m² útiles', '3 habitaciones', '1 baño', 'Balcón', 'Segunda mano/buen estado', 'Armarios empotrados', 'Trastero', 'Amueblado y cocina equipada', 'Planta 3ª exterior', 'Sin ascensor']</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>

</xml_diff>